<commit_message>
FIX SKRIPSI BUAT SIDANG
</commit_message>
<xml_diff>
--- a/Data Curas Kab Probolinggo.xlsx
+++ b/Data Curas Kab Probolinggo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SKRIPSI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CADANGAN SKRIPSI GIT HUB\DATA SKRIPSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B19E3DE-94D8-4477-AD7C-0BF95A452EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8227C8D7-6D6A-422E-B69C-A2B1D296CE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Curas" sheetId="2" r:id="rId2"/>
     <sheet name="Kriminal" sheetId="3" r:id="rId3"/>
-    <sheet name="Lembar1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
+    <sheet name="Lembar1" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="45">
   <si>
     <t xml:space="preserve">Kecamatan </t>
   </si>
@@ -139,13 +140,37 @@
   </si>
   <si>
     <t>Kasus Kriminal 2022</t>
+  </si>
+  <si>
+    <t>Nilai k</t>
+  </si>
+  <si>
+    <t>Nilai SSE</t>
+  </si>
+  <si>
+    <t>Selisih SSE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Aman</t>
+  </si>
+  <si>
+    <t>Sedang</t>
+  </si>
+  <si>
+    <t>Rawan</t>
+  </si>
+  <si>
+    <t>Krenjengan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,16 +178,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -170,11 +218,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -193,6 +276,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2030,7 +2152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEEB2ACC-7E13-4834-965D-558B0C509243}">
   <dimension ref="B5:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -2377,10 +2499,316 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F91B0C-8134-4688-80F8-10EA2BCA3AA6}">
+  <dimension ref="C7:Y32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="3:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="F8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="12">
+        <v>2</v>
+      </c>
+      <c r="H8" s="12">
+        <v>3</v>
+      </c>
+      <c r="I8" s="12">
+        <v>4</v>
+      </c>
+      <c r="J8" s="12">
+        <v>5</v>
+      </c>
+      <c r="K8" s="12">
+        <v>6</v>
+      </c>
+      <c r="L8" s="12">
+        <v>7</v>
+      </c>
+      <c r="M8" s="12">
+        <v>8</v>
+      </c>
+      <c r="N8" s="12">
+        <v>9</v>
+      </c>
+      <c r="O8" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="3:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="F9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="13">
+        <v>575.88</v>
+      </c>
+      <c r="H9" s="14">
+        <v>219214</v>
+      </c>
+      <c r="I9" s="13">
+        <v>74.713999999999999</v>
+      </c>
+      <c r="J9" s="13">
+        <v>74.713999999999999</v>
+      </c>
+      <c r="K9" s="13">
+        <v>74.713999999999999</v>
+      </c>
+      <c r="L9" s="13">
+        <v>53.381</v>
+      </c>
+      <c r="M9" s="13">
+        <v>37.713999999999999</v>
+      </c>
+      <c r="N9" s="13">
+        <v>38.082999999999998</v>
+      </c>
+      <c r="O9" s="13">
+        <v>12.416</v>
+      </c>
+    </row>
+    <row r="10" spans="3:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="F10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="15">
+        <v>356.666</v>
+      </c>
+      <c r="I10" s="13">
+        <v>144.5</v>
+      </c>
+      <c r="J10" s="12">
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="13">
+        <v>21.332999999999998</v>
+      </c>
+      <c r="M10" s="13">
+        <v>15.667</v>
+      </c>
+      <c r="N10" s="13">
+        <v>-0.36899999999999999</v>
+      </c>
+      <c r="O10" s="13">
+        <v>25.667000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="3:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="3:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="3:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="N13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="P13" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q13" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="R13" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="S13" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="T13" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="U13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="V13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="W13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="X13" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y13" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="3:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C14" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="3:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C15" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="3:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C16" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C17" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AFD936-2D16-4187-A336-390F48FE9670}">
   <dimension ref="B2:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>

</xml_diff>